<commit_message>
[feat] add more strategies
</commit_message>
<xml_diff>
--- a/trade_monitoring_2070.xlsx
+++ b/trade_monitoring_2070.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1937,6 +1937,1570 @@
         <v>-2</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>19145859743</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:20:02</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>4</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>71.89999999999964</v>
+      </c>
+      <c r="H45" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>19145863006</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:22:01</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>72.89999999999964</v>
+      </c>
+      <c r="H46" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>19145866013</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:24:02</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>2</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
+        <v>74.89999999999964</v>
+      </c>
+      <c r="H47" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>19145869019</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:26:05</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>4</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>78.89999999999964</v>
+      </c>
+      <c r="H48" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>19145873047</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:28:04</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>8</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G49" t="n">
+        <v>76.5</v>
+      </c>
+      <c r="H49" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>19145876388</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:30:02</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G50" t="n">
+        <v>77.5</v>
+      </c>
+      <c r="H50" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>19145880350</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:32:02</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>2</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G51" t="n">
+        <v>79.5</v>
+      </c>
+      <c r="H51" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>19145884769</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:34:02</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>4</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>78.29999999999927</v>
+      </c>
+      <c r="H52" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>19145888609</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:36:03</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G53" t="n">
+        <v>78</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>19145893134</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:38:03</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G54" t="n">
+        <v>79</v>
+      </c>
+      <c r="H54" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>19145896355</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:40:04</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>2</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G55" t="n">
+        <v>81</v>
+      </c>
+      <c r="H55" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>19145900395</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:42:02</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>4</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G56" t="n">
+        <v>85</v>
+      </c>
+      <c r="H56" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>19145904352</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:44:02</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>8</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G57" t="n">
+        <v>82.60000000000036</v>
+      </c>
+      <c r="H57" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>19145912618</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:48:04</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>1</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G58" t="n">
+        <v>84.60000000000036</v>
+      </c>
+      <c r="H58" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>19145916037</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:50:02</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G59" t="n">
+        <v>84</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.6000000000000001</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>19145920126</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:52:02</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G60" t="n">
+        <v>85</v>
+      </c>
+      <c r="H60" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>19145924197</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:54:02</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>2</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G61" t="n">
+        <v>87</v>
+      </c>
+      <c r="H61" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>19145927684</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:56:03</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>4</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G62" t="n">
+        <v>85.79999999999927</v>
+      </c>
+      <c r="H62" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>19145931353</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>2024-07-18 13:58:02</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>1</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G63" t="n">
+        <v>86.79999999999927</v>
+      </c>
+      <c r="H63" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>19145939487</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:02:04</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>2</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G64" t="n">
+        <v>90.79999999999927</v>
+      </c>
+      <c r="H64" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>19145943216</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:04:03</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>4</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G65" t="n">
+        <v>89.60000000000036</v>
+      </c>
+      <c r="H65" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>19145946578</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:06:03</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G66" t="n">
+        <v>90.60000000000036</v>
+      </c>
+      <c r="H66" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>19145951571</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:08:02</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>2</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>92.60000000000036</v>
+      </c>
+      <c r="H67" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>19145955831</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:10:04</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>4</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G68" t="n">
+        <v>91.39999999999964</v>
+      </c>
+      <c r="H68" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>19145960106</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:12:02</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>1</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G69" t="n">
+        <v>91.10000000000036</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>19145964217</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:14:02</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>92.10000000000036</v>
+      </c>
+      <c r="H70" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>19145968297</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:16:02</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>2</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>94.10000000000036</v>
+      </c>
+      <c r="H71" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>19145972635</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:18:03</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>4</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>98.10000000000036</v>
+      </c>
+      <c r="H72" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>19145976554</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:20:05</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>8</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>106.1000000000004</v>
+      </c>
+      <c r="H73" t="n">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>19145980939</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:22:02</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>16</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>122.1000000000004</v>
+      </c>
+      <c r="H74" t="n">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>19145985409</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:24:02</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>32</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>154.1000000000004</v>
+      </c>
+      <c r="H75" t="n">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>19145989469</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:26:03</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>64</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>218.1000000000004</v>
+      </c>
+      <c r="H76" t="n">
+        <v>-64</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>19145993464</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:28:02</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>217.7999999999993</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>19145997284</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:30:02</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>217.5</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>19146001841</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:32:04</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>1</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>217.2000000000007</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>19146006511</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:34:02</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>1</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>216.8999999999996</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>19146010500</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:36:02</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>1</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>216.6000000000004</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>19146016004</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:38:04</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>1</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>217.6000000000004</v>
+      </c>
+      <c r="H82" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>19146020080</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:40:02</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>2</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>219.6000000000004</v>
+      </c>
+      <c r="H83" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>19146024119</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:42:02</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E84" t="n">
+        <v>4</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>223.6000000000004</v>
+      </c>
+      <c r="H84" t="n">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>19146028242</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:44:04</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E85" t="n">
+        <v>8</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>221.2000000000007</v>
+      </c>
+      <c r="H85" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>19146032419</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:46:02</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E86" t="n">
+        <v>1</v>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>220.8999999999996</v>
+      </c>
+      <c r="H86" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>19146037116</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:48:02</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E87" t="n">
+        <v>1</v>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>220.6000000000004</v>
+      </c>
+      <c r="H87" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>19146040813</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:50:02</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E88" t="n">
+        <v>1</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>221.6000000000004</v>
+      </c>
+      <c r="H88" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>19146045545</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:52:02</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E89" t="n">
+        <v>2</v>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Loss</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
+        <v>224.6000000000004</v>
+      </c>
+      <c r="H89" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>19146050311</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>2024-07-18 14:54:02</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Moving Average Crossover Strategy</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E90" t="n">
+        <v>4</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Win</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>223.3999999999996</v>
+      </c>
+      <c r="H90" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>